<commit_message>
Section 2: Creating with API requests
</commit_message>
<xml_diff>
--- a/Software Testing voortgang.xlsx
+++ b/Software Testing voortgang.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Algemeen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Algemeen\Desktop\School\SoftwareTesting21-22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E3FE3E-5BCE-4956-889C-53DC7E1CEBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D769124E-0866-4110-889D-C1F6A45D3931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Week 1</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Section 1: Introduction and first steps in Postman</t>
+  </si>
+  <si>
+    <t>Section 2: Creating with API requests</t>
   </si>
 </sst>
 </file>
@@ -372,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A13:C16"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,42 +386,48 @@
     <col min="2" max="2" width="55.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C14">
+      <c r="C2">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C15">
+      <c r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Section 10, 12 & 14
</commit_message>
<xml_diff>
--- a/Software Testing voortgang.xlsx
+++ b/Software Testing voortgang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Algemeen\Desktop\School\SoftwareTesting21-22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321FAAF9-9D47-451B-B371-D82582D2B93D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1945FF-2762-4BC9-8757-A98BEC36D8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3855" yWindow="1845" windowWidth="14760" windowHeight="13755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Week 1</t>
   </si>
@@ -106,6 +106,18 @@
   </si>
   <si>
     <t>Section 7&amp;9</t>
+  </si>
+  <si>
+    <t>Section 14: Basic access authentication &amp; Oauth2</t>
+  </si>
+  <si>
+    <t>Section 10 &amp; 12</t>
+  </si>
+  <si>
+    <t>Week 13</t>
+  </si>
+  <si>
+    <t>Week 14</t>
   </si>
 </sst>
 </file>
@@ -429,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,6 +595,28 @@
         <v>8</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>